<commit_message>
Ignore sqlite databases and translation artifacts
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada_totals.xlsx
+++ b/notebooks/jesuita-entrada_totals.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -498,40 +498,40 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>Lisboa</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15340815</t>
+          <t>15460000</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17590310</t>
+          <t>17530612</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Lisboa</t>
+          <t>Paris</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>15460000</t>
+          <t>15340815</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17521123</t>
+          <t>17590310</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -778,7 +778,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Roma (Noviciado de Sant'Andrea al Quirinale)</t>
+          <t>Tournai</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -786,52 +786,52 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>15710816</t>
+          <t>15960705</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>17111213</t>
+          <t>16960929</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Tournai</t>
+          <t>Bordeaux</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>15960705</t>
+          <t>16680920</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>16960929</t>
+          <t>17431107</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Bordeaux</t>
+          <t>Alcalá</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>16680920</t>
+          <t>15550952</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>17431107</t>
+          <t>15710624</t>
         </is>
       </c>
     </row>
@@ -898,27 +898,27 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Lisboa (Arroios)</t>
+          <t>Cracóvia</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>17450423</t>
+          <t>16310816</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>17530612</t>
+          <t>16760909</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Alcalá</t>
+          <t>Lyon</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -926,19 +926,19 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15550952</t>
+          <t>16740927</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>15710624</t>
+          <t>16930923</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Cracóvia</t>
+          <t>Palermo, Sicília</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -946,19 +946,19 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16310816</t>
+          <t>16181103</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>16760909</t>
+          <t>16561022</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Lyon</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -966,59 +966,59 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>16740927</t>
+          <t>15480613</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>16930923</t>
+          <t>16780000</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Palermo, Sicília</t>
+          <t>Bolonha</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16181103</t>
+          <t>16680000</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>16561022</t>
+          <t>17250728</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Hangchow</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>15480613</t>
+          <t>16270000</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>16780000</t>
+          <t>16790621</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Bolonha</t>
+          <t>Milão</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1026,19 +1026,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>16680000</t>
+          <t>16731021</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>17250728</t>
+          <t>16901101</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Hangchow</t>
+          <t>Toulouse</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1046,19 +1046,19 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>16270000</t>
+          <t>16800921</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>16790621</t>
+          <t>17280930</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Milão</t>
+          <t>Trier</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1066,59 +1066,59 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>16731021</t>
+          <t>16770821</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>16901101</t>
+          <t>17271019</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Toulouse</t>
+          <t>Arona</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16800921</t>
+          <t>15960921</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>17280930</t>
+          <t>16140824</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Trier</t>
+          <t>Boémia</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>16770821</t>
+          <t>17290927</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>17271019</t>
+          <t>17291010</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Alcalá de Henares</t>
+          <t>Douai</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1126,19 +1126,19 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15580413</t>
+          <t>15941109</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15710000</t>
+          <t>15990512</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Arona</t>
+          <t>Ferrara</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1146,19 +1146,19 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15960921</t>
+          <t>15550000</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>16140824</t>
+          <t>15561200</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Boémia</t>
+          <t>Leoben</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1166,19 +1166,19 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17290927</t>
+          <t>16871224</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>17291010</t>
+          <t>16881012</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Douai</t>
+          <t>Messina, Sicília</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1186,19 +1186,19 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>15941109</t>
+          <t>15820000</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15990512</t>
+          <t>17061207</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Ferrara</t>
+          <t>Montmartre</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1206,19 +1206,19 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15550000</t>
+          <t>15340815</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15561200</t>
+          <t>15340815</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Leoben</t>
+          <t>Saragoça</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1226,19 +1226,19 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>16871224</t>
+          <t>16740613</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>16881012</t>
+          <t>16771115</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Messina, Sicília</t>
+          <t>Shiuchow</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1246,19 +1246,19 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15820000</t>
+          <t>15910101</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>17061207</t>
+          <t>16050000</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Montmartre</t>
+          <t>Shiuchow, Chao-tcheou fou</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1266,19 +1266,19 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>15340815</t>
+          <t>15891100</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15340815</t>
+          <t>15891100</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Saragoça</t>
+          <t>Vilnius</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1286,59 +1286,59 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>16740613</t>
+          <t>16180531</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>16771115</t>
+          <t>16720811</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Shiuchow, Chao-tcheou fou</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15891100</t>
+          <t>16410000</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>15891100</t>
+          <t>16410000</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Vilnius</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16180531</t>
+          <t>17280105</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>16720811</t>
+          <t>17280105</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Colorno</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1346,19 +1346,19 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>16410000</t>
+          <t>17991116</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>16410000</t>
+          <t>17991116</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Courtrai</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1366,19 +1366,19 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>17280105</t>
+          <t>16440926</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>17280105</t>
+          <t>16440926</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Colorno</t>
+          <t>Goa, Índia</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1386,19 +1386,19 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>17991116</t>
+          <t>15791200</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>17991116</t>
+          <t>15791200</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Courtrai</t>
+          <t>Japão (província)</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1406,19 +1406,19 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16440926</t>
+          <t>17280523</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>16440926</t>
+          <t>17280523</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Goa, Índia</t>
+          <t>Krems</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1426,19 +1426,19 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15791200</t>
+          <t>16641031</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>15791200</t>
+          <t>16641031</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Japão (província)</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1446,19 +1446,19 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>17280523</t>
+          <t>15680711</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>17280523</t>
+          <t>15680711</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Krems</t>
+          <t>Lorette</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1466,19 +1466,19 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>16641031</t>
+          <t>15590425</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>16641031</t>
+          <t>15590425</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Mainz</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1486,19 +1486,19 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15680711</t>
+          <t>16730717</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>15680711</t>
+          <t>16730717</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Lorette</t>
+          <t>Manila</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1506,19 +1506,19 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>15590425</t>
+          <t>16721011</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>15590425</t>
+          <t>16721011</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Mainz</t>
+          <t>Mazowsze (província)</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1526,19 +1526,19 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16730717</t>
+          <t>17700813</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>16730717</t>
+          <t>17700813</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>Manila</t>
+          <t>Milão (província)</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1546,19 +1546,19 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16721011</t>
+          <t>16581105</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>16721011</t>
+          <t>16581105</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Mazowsze (província)</t>
+          <t>Nan-tch'ang</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1566,19 +1566,19 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>17700813</t>
+          <t>16080000</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>17700813</t>
+          <t>16080000</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Milão (província)</t>
+          <t>Nanquim</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1586,19 +1586,19 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16581105</t>
+          <t>16080300</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>16581105</t>
+          <t>16080300</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Nan-tch'ang</t>
+          <t>Novellara</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1606,19 +1606,19 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16080000</t>
+          <t>16001101</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>16080000</t>
+          <t>16001101</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>Nanquim</t>
+          <t>Novellario</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1626,19 +1626,19 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>16080300</t>
+          <t>16170121</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>16080300</t>
+          <t>16170121</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Novellara</t>
+          <t>Ormuz</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1646,19 +1646,19 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>16001101</t>
+          <t>000000</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>16001101</t>
+          <t>000000</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Novellario</t>
+          <t>Ozukio (noviciado)</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1666,19 +1666,19 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>16170121</t>
+          <t>15811100</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>16170121</t>
+          <t>15811100</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>Ormuz</t>
+          <t>Polotsk</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1686,19 +1686,19 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>17860903</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>17860903</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>Ozukio (noviciado)</t>
+          <t>Salamanca</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1706,19 +1706,19 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15811100</t>
+          <t>16830419</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15811100</t>
+          <t>16830419</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Polotsk</t>
+          <t>Shanghai</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1726,19 +1726,19 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>17860903</t>
+          <t>16100000</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>17860903</t>
+          <t>16100000</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>Salamanca</t>
+          <t>Todos-os-Santos, Nagasaki</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1746,19 +1746,19 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16830419</t>
+          <t>16070202</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>16830419</t>
+          <t>16070202</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Shanghai</t>
+          <t>Toulouse (província)</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1766,19 +1766,19 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16100000</t>
+          <t>17500319</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>16100000</t>
+          <t>17500319</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>Shiuchow</t>
+          <t>Trenčín</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1786,19 +1786,19 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>16050000</t>
+          <t>17291027</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>16050000</t>
+          <t>17291027</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Shiuchow (Chao-tcheou)</t>
+          <t>Valença</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1806,19 +1806,19 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>15910101</t>
+          <t>15610927</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>15910101</t>
+          <t>15610927</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>Todos-os-Santos, Nagasaki</t>
+          <t>Veneza</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1826,19 +1826,19 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>16070202</t>
+          <t>17180424</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>16070202</t>
+          <t>17180424</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>Toulouse (província)</t>
+          <t>Villaregio</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1846,19 +1846,19 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>17500319</t>
+          <t>15890406</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>17500319</t>
+          <t>15890406</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>Trenčín</t>
+          <t>[Missão]</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1866,19 +1866,19 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>17291027</t>
+          <t>17310308</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>17291027</t>
+          <t>17310308</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>Valença</t>
+          <t>província do Japão</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1886,19 +1886,19 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>15610927</t>
+          <t>16910113</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>15610927</t>
+          <t>16910113</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>Veneza</t>
+          <t>Índia</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1906,90 +1906,10 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>17180424</t>
+          <t>15530000</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
-        <is>
-          <t>17180424</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>Villaregio</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>1</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>15890406</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>15890406</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>[Missão]</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>1</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>17310308</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>17310308</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>província do Japão</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>1</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>16910113</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>16910113</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>Índia</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>15530000</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
         <is>
           <t>15530000</t>
         </is>

</xml_diff>

<commit_message>
Update notebooks and stats
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada_totals.xlsx
+++ b/notebooks/jesuita-entrada_totals.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Goa, Índia</t>
+          <t>Japão (província)</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1386,19 +1386,19 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>15791200</t>
+          <t>17280523</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>15791200</t>
+          <t>17280523</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Japão (província)</t>
+          <t>Krems</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1406,19 +1406,19 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>17280523</t>
+          <t>16641031</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>17280523</t>
+          <t>16641031</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Krems</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1426,19 +1426,19 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>16641031</t>
+          <t>15680711</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>16641031</t>
+          <t>15680711</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Lorette</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1446,19 +1446,19 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15680711</t>
+          <t>15590425</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>15680711</t>
+          <t>15590425</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Lorette</t>
+          <t>Mainz</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1466,19 +1466,19 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15590425</t>
+          <t>16730717</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15590425</t>
+          <t>16730717</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Mainz</t>
+          <t>Manila</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1486,19 +1486,19 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16730717</t>
+          <t>16721011</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>16730717</t>
+          <t>16721011</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Manila</t>
+          <t>Mazowsze (província)</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1506,19 +1506,19 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16721011</t>
+          <t>17700813</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>16721011</t>
+          <t>17700813</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Mazowsze (província)</t>
+          <t>Milão (província)</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1526,19 +1526,19 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>17700813</t>
+          <t>16581105</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>17700813</t>
+          <t>16581105</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>Milão (província)</t>
+          <t>Nan-tch'ang</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1546,19 +1546,19 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16581105</t>
+          <t>16080000</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>16581105</t>
+          <t>16080000</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Nan-tch'ang</t>
+          <t>Nanquim</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1566,19 +1566,19 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16080000</t>
+          <t>16080300</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>16080000</t>
+          <t>16080300</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Nanquim</t>
+          <t>Novellara</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1586,19 +1586,19 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16080300</t>
+          <t>16001101</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>16080300</t>
+          <t>16001101</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Novellara</t>
+          <t>Novellario</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1606,19 +1606,19 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16001101</t>
+          <t>16170121</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>16001101</t>
+          <t>16170121</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>Novellario</t>
+          <t>Ormuz</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1626,19 +1626,19 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>16170121</t>
+          <t>000000</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>16170121</t>
+          <t>000000</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Ormuz</t>
+          <t>Ozukio (noviciado)</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1646,19 +1646,19 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>15811100</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>15811100</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Ozukio (noviciado)</t>
+          <t>Polotsk</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1666,19 +1666,19 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>15811100</t>
+          <t>17860903</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>15811100</t>
+          <t>17860903</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>Polotsk</t>
+          <t>Salamanca</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1686,19 +1686,19 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>17860903</t>
+          <t>16830419</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>17860903</t>
+          <t>16830419</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>Salamanca</t>
+          <t>Shanghai</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1706,19 +1706,19 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16830419</t>
+          <t>16100000</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>16830419</t>
+          <t>16100000</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Shanghai</t>
+          <t>Todos-os-Santos, Nagasaki</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1726,19 +1726,19 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16100000</t>
+          <t>16070202</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>16100000</t>
+          <t>16070202</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>Todos-os-Santos, Nagasaki</t>
+          <t>Toulouse (província)</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1746,19 +1746,19 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16070202</t>
+          <t>17500319</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>16070202</t>
+          <t>17500319</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Toulouse (província)</t>
+          <t>Trenčín</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1766,19 +1766,19 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>17500319</t>
+          <t>17291027</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>17500319</t>
+          <t>17291027</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>Trenčín</t>
+          <t>Valença</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1786,19 +1786,19 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>17291027</t>
+          <t>15610927</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>17291027</t>
+          <t>15610927</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Valença</t>
+          <t>Veneza</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1806,19 +1806,19 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>15610927</t>
+          <t>17180424</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>15610927</t>
+          <t>17180424</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>Veneza</t>
+          <t>Villaregio</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1826,19 +1826,19 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>17180424</t>
+          <t>15890406</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>17180424</t>
+          <t>15890406</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>Villaregio</t>
+          <t>[Missão]</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1846,19 +1846,19 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>15890406</t>
+          <t>17310308</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>15890406</t>
+          <t>17310308</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>[Missão]</t>
+          <t>província do Japão</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1866,19 +1866,19 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>17310308</t>
+          <t>16910113</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>17310308</t>
+          <t>16910113</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>província do Japão</t>
+          <t>Índia</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1886,30 +1886,10 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16910113</t>
+          <t>15530000</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
-        <is>
-          <t>16910113</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>Índia</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>1</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>15530000</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
         <is>
           <t>15530000</t>
         </is>

</xml_diff>

<commit_message>
Updated notebooks and stats
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada_totals.xlsx
+++ b/notebooks/jesuita-entrada_totals.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>506</v>
+        <v>493</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -498,60 +498,60 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Lisboa</t>
+          <t>Paris</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15460000</t>
+          <t>15340815</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17530612</t>
+          <t>17590310</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>Roma</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>15340815</t>
+          <t>15400927</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17590310</t>
+          <t>17560709</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Roma</t>
+          <t>Lisboa</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>15400927</t>
+          <t>15460000</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>17560709</t>
+          <t>17521123</t>
         </is>
       </c>
     </row>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -858,27 +858,27 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Chieri</t>
+          <t>Lisboa, Arroios</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>16280213</t>
+          <t>17450423</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>16880120</t>
+          <t>17530612</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Japão</t>
+          <t>Chieri</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -886,39 +886,39 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15560000</t>
+          <t>16280213</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>16260600</t>
+          <t>16880120</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Cracóvia</t>
+          <t>Japão</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16310816</t>
+          <t>15560000</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>16760909</t>
+          <t>16260600</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Lyon</t>
+          <t>Cracóvia</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -926,19 +926,19 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>16740927</t>
+          <t>16310816</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>16930923</t>
+          <t>16760909</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Palermo, Sicília</t>
+          <t>Lyon</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -946,19 +946,19 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16181103</t>
+          <t>16740927</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>16561022</t>
+          <t>16930923</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Palermo, Sicília</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -966,39 +966,39 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>15480613</t>
+          <t>16181103</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>16780000</t>
+          <t>16561022</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Bolonha</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16680000</t>
+          <t>15480613</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>17250728</t>
+          <t>16780000</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Hangchow</t>
+          <t>Bolonha</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1006,19 +1006,19 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>16270000</t>
+          <t>16680000</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>16790621</t>
+          <t>17250728</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Milão</t>
+          <t>Hangchow</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1026,19 +1026,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>16731021</t>
+          <t>16270000</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>16901101</t>
+          <t>16790621</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Toulouse</t>
+          <t>Milão</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1046,19 +1046,19 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>16800921</t>
+          <t>16731021</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>17280930</t>
+          <t>16901101</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Trier</t>
+          <t>Toulouse</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1066,39 +1066,39 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>16770821</t>
+          <t>16800921</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>17271019</t>
+          <t>17280930</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Arona</t>
+          <t>Trier</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>15960921</t>
+          <t>16770821</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>16140824</t>
+          <t>17271019</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Boémia</t>
+          <t>Arona</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1106,19 +1106,19 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>17290927</t>
+          <t>15960921</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>17291010</t>
+          <t>16140824</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Douai</t>
+          <t>Boémia</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1126,19 +1126,19 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15941109</t>
+          <t>17290927</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15990512</t>
+          <t>17291010</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Ferrara</t>
+          <t>Douai</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1146,19 +1146,19 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15550000</t>
+          <t>15941109</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15561200</t>
+          <t>15990512</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Leoben</t>
+          <t>Ferrara</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1166,19 +1166,19 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>16871224</t>
+          <t>15550000</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>16881012</t>
+          <t>15561200</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Messina, Sicília</t>
+          <t>Leoben</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1186,19 +1186,19 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>15820000</t>
+          <t>16871224</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>17061207</t>
+          <t>16881012</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Montmartre</t>
+          <t>Messina, Sicília</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1206,19 +1206,19 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15340815</t>
+          <t>15820000</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15340815</t>
+          <t>17061207</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Saragoça</t>
+          <t>Montmartre</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1226,19 +1226,19 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>16740613</t>
+          <t>15340815</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>16771115</t>
+          <t>15340815</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Shiuchow</t>
+          <t>Saragoça</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1246,19 +1246,19 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15910101</t>
+          <t>16740613</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>16050000</t>
+          <t>16771115</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Shiuchow, Chao-tcheou fou</t>
+          <t>Shiuchow</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1266,19 +1266,19 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>15891100</t>
+          <t>15910101</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15891100</t>
+          <t>16050000</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Vilnius</t>
+          <t>Shiuchow, Chao-tcheou fou</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1286,39 +1286,39 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>16180531</t>
+          <t>15891100</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>16720811</t>
+          <t>15891100</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Vilnius</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>16410000</t>
+          <t>16180531</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>16410000</t>
+          <t>16720811</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1326,19 +1326,19 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>17280105</t>
+          <t>16410000</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>17280105</t>
+          <t>16410000</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Colorno</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1346,19 +1346,19 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>17991116</t>
+          <t>17280105</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>17991116</t>
+          <t>17280105</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Courtrai</t>
+          <t>Colorno</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1366,19 +1366,19 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>16440926</t>
+          <t>17991116</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>16440926</t>
+          <t>17991116</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Japão (província)</t>
+          <t>Courtrai</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1386,19 +1386,19 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>17280523</t>
+          <t>16440926</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>17280523</t>
+          <t>16440926</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Krems</t>
+          <t>Japão (província)</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1406,19 +1406,19 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16641031</t>
+          <t>17280523</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>16641031</t>
+          <t>17280523</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Krems</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1426,19 +1426,19 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15680711</t>
+          <t>16641031</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>15680711</t>
+          <t>16641031</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Lorette</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1446,19 +1446,19 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15590425</t>
+          <t>15680711</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>15590425</t>
+          <t>15680711</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Mainz</t>
+          <t>Lorette</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1466,19 +1466,19 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>16730717</t>
+          <t>15590425</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>16730717</t>
+          <t>15590425</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Manila</t>
+          <t>Mainz</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1486,19 +1486,19 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>16721011</t>
+          <t>16730717</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>16721011</t>
+          <t>16730717</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Mazowsze (província)</t>
+          <t>Manila</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1506,19 +1506,19 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>17700813</t>
+          <t>16721011</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>17700813</t>
+          <t>16721011</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Milão (província)</t>
+          <t>Mazowsze (província)</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1526,19 +1526,19 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16581105</t>
+          <t>17700813</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>16581105</t>
+          <t>17700813</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>Nan-tch'ang</t>
+          <t>Milão (província)</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1546,19 +1546,19 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>16080000</t>
+          <t>16581105</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>16080000</t>
+          <t>16581105</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Nanquim</t>
+          <t>Nan-tch'ang</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1566,19 +1566,19 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>16080300</t>
+          <t>16080000</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>16080300</t>
+          <t>16080000</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Novellara</t>
+          <t>Nanquim</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1586,19 +1586,19 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16001101</t>
+          <t>16080300</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>16001101</t>
+          <t>16080300</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Novellario</t>
+          <t>Novellara</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1606,19 +1606,19 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16170121</t>
+          <t>16001101</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>16170121</t>
+          <t>16001101</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>Ormuz</t>
+          <t>Novellario</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1626,19 +1626,19 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>16170121</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>16170121</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Ozukio (noviciado)</t>
+          <t>Ormuz</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1646,19 +1646,19 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>15811100</t>
+          <t>000000</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>15811100</t>
+          <t>000000</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Polotsk</t>
+          <t>Ozukio (noviciado)</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1666,19 +1666,19 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>17860903</t>
+          <t>15811100</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>17860903</t>
+          <t>15811100</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>Salamanca</t>
+          <t>Polotsk</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1686,19 +1686,19 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16830419</t>
+          <t>17860903</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>16830419</t>
+          <t>17860903</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>Shanghai</t>
+          <t>Salamanca</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1706,19 +1706,19 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>16100000</t>
+          <t>16830419</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>16100000</t>
+          <t>16830419</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Todos-os-Santos, Nagasaki</t>
+          <t>Shanghai</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1726,19 +1726,19 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>16070202</t>
+          <t>16100000</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>16070202</t>
+          <t>16100000</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>Toulouse (província)</t>
+          <t>Todos-os-Santos, Nagasaki</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1746,19 +1746,19 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>17500319</t>
+          <t>16070202</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>17500319</t>
+          <t>16070202</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Trenčín</t>
+          <t>Toulouse (província)</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1766,19 +1766,19 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>17291027</t>
+          <t>17500319</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>17291027</t>
+          <t>17500319</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>Valença</t>
+          <t>Trenčín</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1786,19 +1786,19 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>15610927</t>
+          <t>17291027</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>15610927</t>
+          <t>17291027</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Veneza</t>
+          <t>Valença</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1806,19 +1806,19 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>17180424</t>
+          <t>15610927</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>17180424</t>
+          <t>15610927</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>Villaregio</t>
+          <t>Veneza</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1826,19 +1826,19 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>15890406</t>
+          <t>17180424</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>15890406</t>
+          <t>17180424</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>[Missão]</t>
+          <t>Villaregio</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1846,19 +1846,19 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>17310308</t>
+          <t>15890406</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>17310308</t>
+          <t>15890406</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>província do Japão</t>
+          <t>[Missão]</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1866,30 +1866,50 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16910113</t>
+          <t>17310308</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>16910113</t>
+          <t>17310308</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
+          <t>província do Japão</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>16910113</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>16910113</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
           <t>Índia</t>
         </is>
       </c>
-      <c r="B73" t="n">
-        <v>1</v>
-      </c>
-      <c r="C73" t="inlineStr">
+      <c r="B74" t="n">
+        <v>1</v>
+      </c>
+      <c r="C74" t="inlineStr">
         <is>
           <t>15530000</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>15530000</t>
         </is>

</xml_diff>

<commit_message>
Updated notebooks and reports
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada_totals.xlsx
+++ b/notebooks/jesuita-entrada_totals.xlsx
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualização de notebooks e relatórios
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada_totals.xlsx
+++ b/notebooks/jesuita-entrada_totals.xlsx
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>

</xml_diff>